<commit_message>
- modified the definition of sparsity coefficient to be the average sparsity of coefficient matrix - intorduced adaptive sparsity for @dch and @dchperceptron
</commit_message>
<xml_diff>
--- a/output/to_publish/results2.xlsx
+++ b/output/to_publish/results2.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="results2" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
@@ -104,7 +104,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="20" x14ac:knownFonts="1">
     <font>
@@ -625,17 +625,17 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="15" borderId="10" xfId="24" applyBorder="1"/>
-    <xf numFmtId="165" fontId="1" fillId="15" borderId="10" xfId="24" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="15" borderId="10" xfId="24" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="10" xfId="20" applyBorder="1"/>
-    <xf numFmtId="165" fontId="1" fillId="11" borderId="10" xfId="20" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="11" borderId="10" xfId="20" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="15" borderId="10" xfId="24" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="14" fillId="15" borderId="10" xfId="24" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="19" fillId="15" borderId="10" xfId="24" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="1" fillId="33" borderId="10" xfId="24" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="14" fillId="15" borderId="10" xfId="24" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="19" fillId="15" borderId="10" xfId="24" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="33" borderId="10" xfId="24" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="33" borderId="10" xfId="24" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="14" fillId="11" borderId="10" xfId="20" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="14" fillId="11" borderId="10" xfId="20" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -999,8 +999,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="P12" sqref="P12"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="I43" sqref="I43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1200,7 +1200,7 @@
         <v>0.16406999999999999</v>
       </c>
       <c r="L4" s="7">
-        <v>0.25452999999999998</v>
+        <v>0.70923000000000003</v>
       </c>
       <c r="M4" s="6">
         <v>34</v>
@@ -1209,7 +1209,7 @@
         <v>16</v>
       </c>
       <c r="O4" s="16">
-        <f t="shared" ref="O4:O10" si="0">K4*F4</f>
+        <f t="shared" ref="O4:O9" si="0">K4*F4</f>
         <v>15.586649999999999</v>
       </c>
     </row>
@@ -1248,7 +1248,7 @@
         <v>0.12748000000000001</v>
       </c>
       <c r="L5" s="7">
-        <v>0.25888</v>
+        <v>0.70611999999999997</v>
       </c>
       <c r="M5" s="6">
         <v>34</v>
@@ -1601,7 +1601,7 @@
         <v>5.1290000000000002E-2</v>
       </c>
       <c r="L13" s="7">
-        <v>8.6720000000000005E-2</v>
+        <v>0.18210000000000001</v>
       </c>
       <c r="M13" s="6">
         <v>21</v>
@@ -1649,7 +1649,7 @@
         <v>5.747E-2</v>
       </c>
       <c r="L14" s="7">
-        <v>8.5029999999999994E-2</v>
+        <v>0.18221000000000001</v>
       </c>
       <c r="M14" s="6">
         <v>21</v>
@@ -2002,7 +2002,7 @@
         <v>0.39693000000000001</v>
       </c>
       <c r="L22" s="7">
-        <v>0.16231999999999999</v>
+        <v>0.32434000000000002</v>
       </c>
       <c r="M22" s="6">
         <v>30</v>
@@ -2050,7 +2050,7 @@
         <v>0.27012000000000003</v>
       </c>
       <c r="L23" s="7">
-        <v>0.16064000000000001</v>
+        <v>0.32425999999999999</v>
       </c>
       <c r="M23" s="6">
         <v>30</v>
@@ -2355,7 +2355,7 @@
         <v>4.4479999999999999E-2</v>
       </c>
       <c r="L30" s="7">
-        <v>3.9214500000000001</v>
+        <v>5.4715800000000003</v>
       </c>
       <c r="M30" s="6">
         <v>10</v>
@@ -2403,7 +2403,7 @@
         <v>4.3630000000000002E-2</v>
       </c>
       <c r="L31" s="7">
-        <v>3.9123899999999998</v>
+        <v>5.4707499999999998</v>
       </c>
       <c r="M31" s="6">
         <v>10</v>
@@ -2660,7 +2660,7 @@
         <v>2.0129999999999999E-2</v>
       </c>
       <c r="L37" s="7">
-        <v>3.46658</v>
+        <v>5.0435400000000001</v>
       </c>
       <c r="M37" s="6">
         <v>10</v>
@@ -2708,7 +2708,7 @@
         <v>2.095E-2</v>
       </c>
       <c r="L38" s="7">
-        <v>3.4836</v>
+        <v>5.0436800000000002</v>
       </c>
       <c r="M38" s="6">
         <v>10</v>

</xml_diff>

<commit_message>
- included the KSVD toolbox in the library - cleaned up code for adaptive sparsity - generated results for adaptive sparsity
</commit_message>
<xml_diff>
--- a/output/to_publish/results2.xlsx
+++ b/output/to_publish/results2.xlsx
@@ -106,7 +106,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -250,12 +250,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="34">
     <fill>
@@ -439,7 +433,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -619,7 +613,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -632,9 +626,6 @@
     <xf numFmtId="164" fontId="1" fillId="11" borderId="10" xfId="20" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="15" borderId="10" xfId="24" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="14" fillId="15" borderId="10" xfId="24" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="19" fillId="15" borderId="10" xfId="24" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="1" fillId="33" borderId="10" xfId="24" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="33" borderId="10" xfId="24" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="14" fillId="11" borderId="10" xfId="20" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -642,6 +633,7 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="1" fillId="11" borderId="10" xfId="20" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="1" fillId="15" borderId="10" xfId="24" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="33" borderId="10" xfId="24" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -999,8 +991,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="I43" sqref="I43"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="H45" sqref="H45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1015,11 +1007,11 @@
     <col min="8" max="8" width="12.44140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="16.33203125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.77734375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="21.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.44140625" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="21.44140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.77734375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.3">
@@ -1056,17 +1048,17 @@
       <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="O1" s="14" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.3">
@@ -1103,18 +1095,18 @@
       <c r="K2" s="7">
         <v>6.2100000000000002E-3</v>
       </c>
-      <c r="L2" s="7">
-        <v>0.70232000000000006</v>
-      </c>
-      <c r="M2" s="6">
-        <v>1</v>
-      </c>
-      <c r="N2" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="O2" s="16">
+      <c r="L2" s="13">
         <f>K2*F2</f>
         <v>0.99981000000000009</v>
+      </c>
+      <c r="M2" s="7">
+        <v>0.70232000000000006</v>
+      </c>
+      <c r="N2" s="6">
+        <v>1</v>
+      </c>
+      <c r="O2" s="6" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
@@ -1151,18 +1143,18 @@
       <c r="K3" s="7">
         <v>1.3820000000000001E-2</v>
       </c>
-      <c r="L3" s="7">
-        <v>0.70867000000000002</v>
-      </c>
-      <c r="M3" s="6">
-        <v>2</v>
-      </c>
-      <c r="N3" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="O3" s="16">
+      <c r="L3" s="13">
         <f>K3*F3</f>
         <v>1.6584000000000001</v>
+      </c>
+      <c r="M3" s="7">
+        <v>0.70867000000000002</v>
+      </c>
+      <c r="N3" s="6">
+        <v>2</v>
+      </c>
+      <c r="O3" s="6" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
@@ -1190,7 +1182,7 @@
       <c r="H4" s="6">
         <v>13726</v>
       </c>
-      <c r="I4" s="13">
+      <c r="I4" s="10">
         <v>1.1501600000000001</v>
       </c>
       <c r="J4" s="6">
@@ -1199,18 +1191,18 @@
       <c r="K4" s="7">
         <v>0.16406999999999999</v>
       </c>
-      <c r="L4" s="7">
+      <c r="L4" s="13">
+        <f>K4*F4</f>
+        <v>15.586649999999999</v>
+      </c>
+      <c r="M4" s="7">
         <v>0.70923000000000003</v>
       </c>
-      <c r="M4" s="6">
+      <c r="N4" s="6">
         <v>34</v>
       </c>
-      <c r="N4" s="6" t="s">
+      <c r="O4" s="6" t="s">
         <v>16</v>
-      </c>
-      <c r="O4" s="16">
-        <f t="shared" ref="O4:O9" si="0">K4*F4</f>
-        <v>15.586649999999999</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
@@ -1236,10 +1228,10 @@
         <v>11934</v>
       </c>
       <c r="H5" s="6">
-        <v>7308</v>
+        <v>11163</v>
       </c>
       <c r="I5" s="7">
-        <v>0.61236999999999997</v>
+        <v>0.93539000000000005</v>
       </c>
       <c r="J5" s="6">
         <v>16</v>
@@ -1247,18 +1239,18 @@
       <c r="K5" s="7">
         <v>0.12748000000000001</v>
       </c>
-      <c r="L5" s="7">
+      <c r="L5" s="13">
+        <f>K5*F5</f>
+        <v>11.983120000000001</v>
+      </c>
+      <c r="M5" s="7">
         <v>0.70611999999999997</v>
       </c>
-      <c r="M5" s="6">
+      <c r="N5" s="6">
         <v>34</v>
       </c>
-      <c r="N5" s="6" t="s">
+      <c r="O5" s="6" t="s">
         <v>16</v>
-      </c>
-      <c r="O5" s="16">
-        <f t="shared" si="0"/>
-        <v>11.983120000000001</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
@@ -1295,18 +1287,18 @@
       <c r="K6" s="5">
         <v>7.7499999999999999E-3</v>
       </c>
-      <c r="L6" s="5">
+      <c r="L6" s="14">
+        <f>K6*F6</f>
+        <v>0.99975000000000003</v>
+      </c>
+      <c r="M6" s="5">
         <v>0.43046000000000001</v>
       </c>
-      <c r="M6" s="4">
+      <c r="N6" s="4">
         <v>1</v>
       </c>
-      <c r="N6" s="4" t="s">
+      <c r="O6" s="4" t="s">
         <v>17</v>
-      </c>
-      <c r="O6" s="17">
-        <f t="shared" si="0"/>
-        <v>0.99975000000000003</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.3">
@@ -1343,18 +1335,18 @@
       <c r="K7" s="5">
         <v>2.4549999999999999E-2</v>
       </c>
-      <c r="L7" s="5">
+      <c r="L7" s="14">
+        <f>K7*F7</f>
+        <v>1.7921499999999999</v>
+      </c>
+      <c r="M7" s="5">
         <v>0.56023000000000001</v>
       </c>
-      <c r="M7" s="4">
+      <c r="N7" s="4">
         <v>2</v>
       </c>
-      <c r="N7" s="4" t="s">
+      <c r="O7" s="4" t="s">
         <v>17</v>
-      </c>
-      <c r="O7" s="17">
-        <f t="shared" si="0"/>
-        <v>1.7921499999999999</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.3">
@@ -1391,18 +1383,18 @@
       <c r="K8" s="5">
         <v>0.1091</v>
       </c>
-      <c r="L8" s="5">
+      <c r="L8" s="14">
+        <f>K8*F8</f>
+        <v>3.7094</v>
+      </c>
+      <c r="M8" s="5">
         <v>0.70399999999999996</v>
       </c>
-      <c r="M8" s="4">
+      <c r="N8" s="4">
         <v>34</v>
       </c>
-      <c r="N8" s="4" t="s">
+      <c r="O8" s="4" t="s">
         <v>17</v>
-      </c>
-      <c r="O8" s="17">
-        <f t="shared" si="0"/>
-        <v>3.7094</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.3">
@@ -1428,10 +1420,10 @@
         <v>11934</v>
       </c>
       <c r="H9" s="4">
-        <v>3375</v>
+        <v>5277</v>
       </c>
       <c r="I9" s="5">
-        <v>0.28281000000000001</v>
+        <v>0.44218000000000002</v>
       </c>
       <c r="J9" s="4">
         <v>7</v>
@@ -1439,18 +1431,18 @@
       <c r="K9" s="5">
         <v>0.18879000000000001</v>
       </c>
-      <c r="L9" s="5">
+      <c r="L9" s="14">
+        <f>K9*F9</f>
+        <v>6.4188600000000005</v>
+      </c>
+      <c r="M9" s="5">
         <v>0.70221</v>
       </c>
-      <c r="M9" s="4">
+      <c r="N9" s="4">
         <v>34</v>
       </c>
-      <c r="N9" s="4" t="s">
+      <c r="O9" s="4" t="s">
         <v>17</v>
-      </c>
-      <c r="O9" s="17">
-        <f t="shared" si="0"/>
-        <v>6.4188600000000005</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.3">
@@ -1465,10 +1457,10 @@
       <c r="I10" s="3"/>
       <c r="J10" s="2"/>
       <c r="K10" s="3"/>
-      <c r="L10" s="3"/>
-      <c r="M10" s="2"/>
+      <c r="L10" s="12"/>
+      <c r="M10" s="3"/>
       <c r="N10" s="2"/>
-      <c r="O10" s="15"/>
+      <c r="O10" s="2"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
@@ -1504,18 +1496,18 @@
       <c r="K11" s="7">
         <v>7.1000000000000002E-4</v>
       </c>
-      <c r="L11" s="7">
-        <v>0.18228</v>
-      </c>
-      <c r="M11" s="6">
-        <v>1</v>
-      </c>
-      <c r="N11" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="O11" s="16">
+      <c r="L11" s="13">
         <f>K11*F11</f>
         <v>1.00607</v>
+      </c>
+      <c r="M11" s="7">
+        <v>0.18228</v>
+      </c>
+      <c r="N11" s="6">
+        <v>1</v>
+      </c>
+      <c r="O11" s="6" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.3">
@@ -1552,18 +1544,18 @@
       <c r="K12" s="7">
         <v>2.7100000000000002E-3</v>
       </c>
-      <c r="L12" s="7">
+      <c r="L12" s="13">
+        <f>K12*F12</f>
+        <v>1.7018800000000001</v>
+      </c>
+      <c r="M12" s="7">
         <v>0.18243000000000001</v>
       </c>
-      <c r="M12" s="6">
+      <c r="N12" s="6">
         <v>2</v>
       </c>
-      <c r="N12" s="6" t="s">
+      <c r="O12" s="6" t="s">
         <v>16</v>
-      </c>
-      <c r="O12" s="16">
-        <f t="shared" ref="O12:O41" si="1">K12*F12</f>
-        <v>1.7018800000000001</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.3">
@@ -1591,7 +1583,7 @@
       <c r="H13" s="6">
         <v>80246</v>
       </c>
-      <c r="I13" s="13">
+      <c r="I13" s="10">
         <v>1.79738</v>
       </c>
       <c r="J13" s="6">
@@ -1600,18 +1592,18 @@
       <c r="K13" s="7">
         <v>5.1290000000000002E-2</v>
       </c>
-      <c r="L13" s="7">
+      <c r="L13" s="13">
+        <f>K13*F13</f>
+        <v>17.74634</v>
+      </c>
+      <c r="M13" s="7">
         <v>0.18210000000000001</v>
       </c>
-      <c r="M13" s="6">
+      <c r="N13" s="6">
         <v>21</v>
       </c>
-      <c r="N13" s="6" t="s">
+      <c r="O13" s="6" t="s">
         <v>16</v>
-      </c>
-      <c r="O13" s="16">
-        <f t="shared" si="1"/>
-        <v>17.74634</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.3">
@@ -1637,10 +1629,10 @@
         <v>44646</v>
       </c>
       <c r="H14" s="6">
-        <v>44646</v>
-      </c>
-      <c r="I14" s="13">
-        <v>1</v>
+        <v>80886</v>
+      </c>
+      <c r="I14" s="10">
+        <v>1.81172</v>
       </c>
       <c r="J14" s="6">
         <v>21</v>
@@ -1648,18 +1640,18 @@
       <c r="K14" s="7">
         <v>5.747E-2</v>
       </c>
-      <c r="L14" s="7">
+      <c r="L14" s="13">
+        <f>K14*F14</f>
+        <v>18.045580000000001</v>
+      </c>
+      <c r="M14" s="7">
         <v>0.18221000000000001</v>
       </c>
-      <c r="M14" s="6">
+      <c r="N14" s="6">
         <v>21</v>
       </c>
-      <c r="N14" s="6" t="s">
+      <c r="O14" s="6" t="s">
         <v>16</v>
-      </c>
-      <c r="O14" s="16">
-        <f t="shared" si="1"/>
-        <v>18.045580000000001</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.3">
@@ -1696,18 +1688,18 @@
       <c r="K15" s="5">
         <v>1.0399999999999999E-3</v>
       </c>
-      <c r="L15" s="5">
+      <c r="L15" s="14">
+        <f>K15*F15</f>
+        <v>1.00464</v>
+      </c>
+      <c r="M15" s="5">
         <v>9.9529999999999993E-2</v>
       </c>
-      <c r="M15" s="4">
+      <c r="N15" s="4">
         <v>1</v>
       </c>
-      <c r="N15" s="4" t="s">
+      <c r="O15" s="4" t="s">
         <v>17</v>
-      </c>
-      <c r="O15" s="17">
-        <f t="shared" si="1"/>
-        <v>1.00464</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.3">
@@ -1744,18 +1736,18 @@
       <c r="K16" s="5">
         <v>6.4700000000000001E-3</v>
       </c>
-      <c r="L16" s="5">
+      <c r="L16" s="14">
+        <f>K16*F16</f>
+        <v>1.8633600000000001</v>
+      </c>
+      <c r="M16" s="5">
         <v>0.15731999999999999</v>
       </c>
-      <c r="M16" s="4">
+      <c r="N16" s="4">
         <v>2</v>
       </c>
-      <c r="N16" s="4" t="s">
+      <c r="O16" s="4" t="s">
         <v>17</v>
-      </c>
-      <c r="O16" s="17">
-        <f t="shared" si="1"/>
-        <v>1.8633600000000001</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.3">
@@ -1792,18 +1784,18 @@
       <c r="K17" s="5">
         <v>0.15668000000000001</v>
       </c>
-      <c r="L17" s="5">
+      <c r="L17" s="14">
+        <f>K17*F17</f>
+        <v>13.474480000000002</v>
+      </c>
+      <c r="M17" s="5">
         <v>0.18237999999999999</v>
       </c>
-      <c r="M17" s="4">
+      <c r="N17" s="4">
         <v>21</v>
       </c>
-      <c r="N17" s="4" t="s">
+      <c r="O17" s="4" t="s">
         <v>17</v>
-      </c>
-      <c r="O17" s="17">
-        <f t="shared" si="1"/>
-        <v>13.474480000000002</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.3">
@@ -1829,10 +1821,10 @@
         <v>44646</v>
       </c>
       <c r="H18" s="4">
-        <v>30303</v>
-      </c>
-      <c r="I18" s="10">
-        <v>0.67874000000000001</v>
+        <v>56940</v>
+      </c>
+      <c r="I18" s="9">
+        <v>1.2753699999999999</v>
       </c>
       <c r="J18" s="4">
         <v>14</v>
@@ -1840,18 +1832,18 @@
       <c r="K18" s="5">
         <v>0.1757</v>
       </c>
-      <c r="L18" s="5">
+      <c r="L18" s="14">
+        <f>K18*F18</f>
+        <v>13.5289</v>
+      </c>
+      <c r="M18" s="5">
         <v>0.18132999999999999</v>
       </c>
-      <c r="M18" s="4">
+      <c r="N18" s="4">
         <v>21</v>
       </c>
-      <c r="N18" s="4" t="s">
+      <c r="O18" s="4" t="s">
         <v>17</v>
-      </c>
-      <c r="O18" s="17">
-        <f t="shared" si="1"/>
-        <v>13.5289</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.3">
@@ -1866,10 +1858,10 @@
       <c r="I19" s="3"/>
       <c r="J19" s="2"/>
       <c r="K19" s="3"/>
-      <c r="L19" s="3"/>
-      <c r="M19" s="2"/>
+      <c r="L19" s="12"/>
+      <c r="M19" s="3"/>
       <c r="N19" s="2"/>
-      <c r="O19" s="15"/>
+      <c r="O19" s="2"/>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A20" s="6" t="s">
@@ -1905,18 +1897,18 @@
       <c r="K20" s="7">
         <v>3.0400000000000002E-3</v>
       </c>
-      <c r="L20" s="7">
+      <c r="L20" s="13">
+        <f>K20*F20</f>
+        <v>1.0001600000000002</v>
+      </c>
+      <c r="M20" s="7">
         <v>0.32429999999999998</v>
       </c>
-      <c r="M20" s="6">
+      <c r="N20" s="6">
         <v>1</v>
       </c>
-      <c r="N20" s="6" t="s">
+      <c r="O20" s="6" t="s">
         <v>16</v>
-      </c>
-      <c r="O20" s="16">
-        <f t="shared" si="1"/>
-        <v>1.0001600000000002</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.3">
@@ -1953,18 +1945,18 @@
       <c r="K21" s="7">
         <v>1.711E-2</v>
       </c>
-      <c r="L21" s="7">
+      <c r="L21" s="13">
+        <f>K21*F21</f>
+        <v>1.81366</v>
+      </c>
+      <c r="M21" s="7">
         <v>0.32356000000000001</v>
       </c>
-      <c r="M21" s="6">
+      <c r="N21" s="6">
         <v>2</v>
       </c>
-      <c r="N21" s="6" t="s">
+      <c r="O21" s="6" t="s">
         <v>16</v>
-      </c>
-      <c r="O21" s="16">
-        <f t="shared" si="1"/>
-        <v>1.81366</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.3">
@@ -1992,7 +1984,7 @@
       <c r="H22" s="6">
         <v>28754</v>
       </c>
-      <c r="I22" s="13">
+      <c r="I22" s="10">
         <v>1.68448</v>
       </c>
       <c r="J22" s="6">
@@ -2001,18 +1993,18 @@
       <c r="K22" s="7">
         <v>0.39693000000000001</v>
       </c>
-      <c r="L22" s="7">
+      <c r="L22" s="13">
+        <f>K22*F22</f>
+        <v>24.212730000000001</v>
+      </c>
+      <c r="M22" s="7">
         <v>0.32434000000000002</v>
       </c>
-      <c r="M22" s="6">
+      <c r="N22" s="6">
         <v>30</v>
       </c>
-      <c r="N22" s="6" t="s">
+      <c r="O22" s="6" t="s">
         <v>16</v>
-      </c>
-      <c r="O22" s="16">
-        <f t="shared" si="1"/>
-        <v>24.212730000000001</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.3">
@@ -2038,10 +2030,10 @@
         <v>17070</v>
       </c>
       <c r="H23" s="6">
-        <v>10962</v>
-      </c>
-      <c r="I23" s="7">
-        <v>0.64217999999999997</v>
+        <v>19615</v>
+      </c>
+      <c r="I23" s="10">
+        <v>1.1490899999999999</v>
       </c>
       <c r="J23" s="6">
         <v>18</v>
@@ -2049,18 +2041,18 @@
       <c r="K23" s="7">
         <v>0.27012000000000003</v>
       </c>
-      <c r="L23" s="7">
+      <c r="L23" s="13">
+        <f>K23*F23</f>
+        <v>16.2072</v>
+      </c>
+      <c r="M23" s="7">
         <v>0.32425999999999999</v>
       </c>
-      <c r="M23" s="6">
+      <c r="N23" s="6">
         <v>30</v>
       </c>
-      <c r="N23" s="6" t="s">
+      <c r="O23" s="6" t="s">
         <v>16</v>
-      </c>
-      <c r="O23" s="16">
-        <f t="shared" si="1"/>
-        <v>16.2072</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.3">
@@ -2097,18 +2089,18 @@
       <c r="K24" s="5">
         <v>4.4999999999999997E-3</v>
       </c>
-      <c r="L24" s="5">
+      <c r="L24" s="14">
+        <f>K24*F24</f>
+        <v>0.99899999999999989</v>
+      </c>
+      <c r="M24" s="5">
         <v>0.19675999999999999</v>
       </c>
-      <c r="M24" s="4">
+      <c r="N24" s="4">
         <v>1</v>
       </c>
-      <c r="N24" s="4" t="s">
+      <c r="O24" s="4" t="s">
         <v>17</v>
-      </c>
-      <c r="O24" s="17">
-        <f t="shared" si="1"/>
-        <v>0.99899999999999989</v>
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.3">
@@ -2145,18 +2137,18 @@
       <c r="K25" s="5">
         <v>5.0869999999999999E-2</v>
       </c>
-      <c r="L25" s="5">
+      <c r="L25" s="14">
+        <f>K25*F25</f>
+        <v>1.93306</v>
+      </c>
+      <c r="M25" s="5">
         <v>0.30113000000000001</v>
       </c>
-      <c r="M25" s="4">
+      <c r="N25" s="4">
         <v>2</v>
       </c>
-      <c r="N25" s="4" t="s">
+      <c r="O25" s="4" t="s">
         <v>17</v>
-      </c>
-      <c r="O25" s="17">
-        <f t="shared" si="1"/>
-        <v>1.93306</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.3">
@@ -2193,18 +2185,18 @@
       <c r="K26" s="5">
         <v>0.38769999999999999</v>
       </c>
-      <c r="L26" s="5">
+      <c r="L26" s="14">
+        <f>K26*F26</f>
+        <v>7.7539999999999996</v>
+      </c>
+      <c r="M26" s="5">
         <v>0.32207000000000002</v>
       </c>
-      <c r="M26" s="4">
+      <c r="N26" s="4">
         <v>30</v>
       </c>
-      <c r="N26" s="4" t="s">
+      <c r="O26" s="4" t="s">
         <v>17</v>
-      </c>
-      <c r="O26" s="17">
-        <f t="shared" si="1"/>
-        <v>7.7539999999999996</v>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.3">
@@ -2230,10 +2222,10 @@
         <v>17070</v>
       </c>
       <c r="H27" s="4">
-        <v>7152</v>
+        <v>13213</v>
       </c>
       <c r="I27" s="5">
-        <v>0.41898000000000002</v>
+        <v>0.77405000000000002</v>
       </c>
       <c r="J27" s="4">
         <v>12</v>
@@ -2241,18 +2233,18 @@
       <c r="K27" s="5">
         <v>0.64732999999999996</v>
       </c>
-      <c r="L27" s="5">
+      <c r="L27" s="14">
+        <f>K27*F27</f>
+        <v>11.65194</v>
+      </c>
+      <c r="M27" s="5">
         <v>0.32396000000000003</v>
       </c>
-      <c r="M27" s="4">
+      <c r="N27" s="4">
         <v>30</v>
       </c>
-      <c r="N27" s="4" t="s">
+      <c r="O27" s="4" t="s">
         <v>17</v>
-      </c>
-      <c r="O27" s="17">
-        <f t="shared" si="1"/>
-        <v>11.65194</v>
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.3">
@@ -2267,10 +2259,10 @@
       <c r="I28" s="3"/>
       <c r="J28" s="2"/>
       <c r="K28" s="3"/>
-      <c r="L28" s="3"/>
-      <c r="M28" s="2"/>
+      <c r="L28" s="12"/>
+      <c r="M28" s="3"/>
       <c r="N28" s="2"/>
-      <c r="O28" s="15"/>
+      <c r="O28" s="2"/>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A29" s="6" t="s">
@@ -2306,18 +2298,18 @@
       <c r="K29" s="7">
         <v>1.3799999999999999E-3</v>
       </c>
-      <c r="L29" s="7">
+      <c r="L29" s="13">
+        <f>K29*F29</f>
+        <v>0.99773999999999996</v>
+      </c>
+      <c r="M29" s="7">
         <v>5.4710000000000001</v>
       </c>
-      <c r="M29" s="6">
+      <c r="N29" s="6">
         <v>10</v>
       </c>
-      <c r="N29" s="6" t="s">
+      <c r="O29" s="6" t="s">
         <v>16</v>
-      </c>
-      <c r="O29" s="16">
-        <f t="shared" si="1"/>
-        <v>0.99773999999999996</v>
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.3">
@@ -2354,18 +2346,18 @@
       <c r="K30" s="7">
         <v>4.4479999999999999E-2</v>
       </c>
-      <c r="L30" s="7">
+      <c r="L30" s="13">
+        <f>K30*F30</f>
+        <v>8.3177599999999998</v>
+      </c>
+      <c r="M30" s="7">
         <v>5.4715800000000003</v>
       </c>
-      <c r="M30" s="6">
+      <c r="N30" s="6">
         <v>10</v>
       </c>
-      <c r="N30" s="6" t="s">
+      <c r="O30" s="6" t="s">
         <v>16</v>
-      </c>
-      <c r="O30" s="16">
-        <f t="shared" si="1"/>
-        <v>8.3177599999999998</v>
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.3">
@@ -2391,10 +2383,10 @@
         <v>784000</v>
       </c>
       <c r="H31" s="6">
-        <v>157060</v>
+        <v>164350</v>
       </c>
       <c r="I31" s="7">
-        <v>0.20033000000000001</v>
+        <v>0.20960000000000001</v>
       </c>
       <c r="J31" s="6">
         <v>10</v>
@@ -2402,18 +2394,18 @@
       <c r="K31" s="7">
         <v>4.3630000000000002E-2</v>
       </c>
-      <c r="L31" s="7">
+      <c r="L31" s="13">
+        <f>K31*F31</f>
+        <v>8.2896999999999998</v>
+      </c>
+      <c r="M31" s="7">
         <v>5.4707499999999998</v>
       </c>
-      <c r="M31" s="6">
+      <c r="N31" s="6">
         <v>10</v>
       </c>
-      <c r="N31" s="6" t="s">
+      <c r="O31" s="6" t="s">
         <v>16</v>
-      </c>
-      <c r="O31" s="16">
-        <f t="shared" si="1"/>
-        <v>8.2896999999999998</v>
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.3">
@@ -2450,18 +2442,18 @@
       <c r="K32" s="5">
         <v>2.1099999999999999E-3</v>
       </c>
-      <c r="L32" s="5">
+      <c r="L32" s="14">
+        <f>K32*F32</f>
+        <v>0.99802999999999997</v>
+      </c>
+      <c r="M32" s="5">
         <v>2.8822999999999999</v>
       </c>
-      <c r="M32" s="4">
+      <c r="N32" s="4">
         <v>10</v>
       </c>
-      <c r="N32" s="4" t="s">
+      <c r="O32" s="4" t="s">
         <v>17</v>
-      </c>
-      <c r="O32" s="17">
-        <f t="shared" si="1"/>
-        <v>0.99802999999999997</v>
       </c>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.3">
@@ -2489,7 +2481,7 @@
       <c r="H33" s="4">
         <v>64204</v>
       </c>
-      <c r="I33" s="11">
+      <c r="I33" s="15">
         <v>8.1890000000000004E-2</v>
       </c>
       <c r="J33" s="4">
@@ -2498,18 +2490,18 @@
       <c r="K33" s="5">
         <v>3.7470000000000003E-2</v>
       </c>
-      <c r="L33" s="5">
+      <c r="L33" s="14">
+        <f>K33*F33</f>
+        <v>2.8477200000000003</v>
+      </c>
+      <c r="M33" s="5">
         <v>5.30769</v>
       </c>
-      <c r="M33" s="4">
+      <c r="N33" s="4">
         <v>10</v>
       </c>
-      <c r="N33" s="4" t="s">
+      <c r="O33" s="4" t="s">
         <v>17</v>
-      </c>
-      <c r="O33" s="17">
-        <f t="shared" si="1"/>
-        <v>2.8477200000000003</v>
       </c>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.3">
@@ -2535,10 +2527,10 @@
         <v>784000</v>
       </c>
       <c r="H34" s="4">
-        <v>66261</v>
-      </c>
-      <c r="I34" s="11">
-        <v>8.4519999999999998E-2</v>
+        <v>68099</v>
+      </c>
+      <c r="I34" s="15">
+        <v>8.6999999999999994E-2</v>
       </c>
       <c r="J34" s="4">
         <v>3</v>
@@ -2546,18 +2538,18 @@
       <c r="K34" s="5">
         <v>3.5040000000000002E-2</v>
       </c>
-      <c r="L34" s="5">
+      <c r="L34" s="14">
+        <f>K34*F34</f>
+        <v>2.8382400000000003</v>
+      </c>
+      <c r="M34" s="5">
         <v>5.4662199999999999</v>
       </c>
-      <c r="M34" s="4">
+      <c r="N34" s="4">
         <v>10</v>
       </c>
-      <c r="N34" s="4" t="s">
+      <c r="O34" s="4" t="s">
         <v>17</v>
-      </c>
-      <c r="O34" s="17">
-        <f t="shared" si="1"/>
-        <v>2.8382400000000003</v>
       </c>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.3">
@@ -2572,10 +2564,10 @@
       <c r="I35" s="3"/>
       <c r="J35" s="2"/>
       <c r="K35" s="3"/>
-      <c r="L35" s="3"/>
-      <c r="M35" s="2"/>
+      <c r="L35" s="12"/>
+      <c r="M35" s="3"/>
       <c r="N35" s="2"/>
-      <c r="O35" s="15"/>
+      <c r="O35" s="2"/>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A36" s="6" t="s">
@@ -2611,18 +2603,18 @@
       <c r="K36" s="7">
         <v>6.7000000000000002E-4</v>
       </c>
-      <c r="L36" s="7">
+      <c r="L36" s="13">
+        <f>K36*F36</f>
+        <v>0.99763000000000002</v>
+      </c>
+      <c r="M36" s="7">
         <v>5.0403200000000004</v>
       </c>
-      <c r="M36" s="6">
+      <c r="N36" s="6">
         <v>10</v>
       </c>
-      <c r="N36" s="6" t="s">
+      <c r="O36" s="6" t="s">
         <v>16</v>
-      </c>
-      <c r="O36" s="16">
-        <f t="shared" si="1"/>
-        <v>0.99763000000000002</v>
       </c>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.3">
@@ -2659,18 +2651,18 @@
       <c r="K37" s="7">
         <v>2.0129999999999999E-2</v>
       </c>
-      <c r="L37" s="7">
+      <c r="L37" s="13">
+        <f>K37*F37</f>
+        <v>8.1727799999999995</v>
+      </c>
+      <c r="M37" s="7">
         <v>5.0435400000000001</v>
       </c>
-      <c r="M37" s="6">
+      <c r="N37" s="6">
         <v>10</v>
       </c>
-      <c r="N37" s="6" t="s">
+      <c r="O37" s="6" t="s">
         <v>16</v>
-      </c>
-      <c r="O37" s="16">
-        <f t="shared" si="1"/>
-        <v>8.1727799999999995</v>
       </c>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.3">
@@ -2696,10 +2688,10 @@
         <v>1568000</v>
       </c>
       <c r="H38" s="6">
-        <v>324182</v>
+        <v>338645</v>
       </c>
       <c r="I38" s="7">
-        <v>0.20674999999999999</v>
+        <v>0.21597</v>
       </c>
       <c r="J38" s="6">
         <v>10</v>
@@ -2707,18 +2699,18 @@
       <c r="K38" s="7">
         <v>2.095E-2</v>
       </c>
-      <c r="L38" s="7">
+      <c r="L38" s="13">
+        <f>K38*F38</f>
+        <v>8.2333499999999997</v>
+      </c>
+      <c r="M38" s="7">
         <v>5.0436800000000002</v>
       </c>
-      <c r="M38" s="6">
+      <c r="N38" s="6">
         <v>10</v>
       </c>
-      <c r="N38" s="6" t="s">
+      <c r="O38" s="6" t="s">
         <v>16</v>
-      </c>
-      <c r="O38" s="16">
-        <f t="shared" si="1"/>
-        <v>8.2333499999999997</v>
       </c>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.3">
@@ -2746,7 +2738,7 @@
       <c r="H39" s="4">
         <v>841376</v>
       </c>
-      <c r="I39" s="4">
+      <c r="I39" s="5">
         <v>0.53659000000000001</v>
       </c>
       <c r="J39" s="4">
@@ -2755,18 +2747,18 @@
       <c r="K39" s="4">
         <v>9.3000000000000005E-4</v>
       </c>
-      <c r="L39" s="4">
+      <c r="L39" s="14">
+        <f>K39*F39</f>
+        <v>0.99696000000000007</v>
+      </c>
+      <c r="M39" s="5">
         <v>2.31934</v>
       </c>
-      <c r="M39" s="4">
+      <c r="N39" s="4">
         <v>10</v>
       </c>
-      <c r="N39" s="4" t="s">
+      <c r="O39" s="4" t="s">
         <v>17</v>
-      </c>
-      <c r="O39" s="17">
-        <f t="shared" si="1"/>
-        <v>0.99696000000000007</v>
       </c>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.3">
@@ -2794,7 +2786,7 @@
       <c r="H40" s="4">
         <v>150999</v>
       </c>
-      <c r="I40" s="12">
+      <c r="I40" s="15">
         <v>9.6299999999999997E-2</v>
       </c>
       <c r="J40" s="4">
@@ -2803,18 +2795,18 @@
       <c r="K40" s="4">
         <v>1.5570000000000001E-2</v>
       </c>
-      <c r="L40" s="4">
+      <c r="L40" s="14">
+        <f>K40*F40</f>
+        <v>2.8181700000000003</v>
+      </c>
+      <c r="M40" s="5">
         <v>4.8726700000000003</v>
       </c>
-      <c r="M40" s="4">
+      <c r="N40" s="4">
         <v>10</v>
       </c>
-      <c r="N40" s="4" t="s">
+      <c r="O40" s="4" t="s">
         <v>17</v>
-      </c>
-      <c r="O40" s="17">
-        <f t="shared" si="1"/>
-        <v>2.8181700000000003</v>
       </c>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.3">
@@ -2840,10 +2832,10 @@
         <v>1568000</v>
       </c>
       <c r="H41" s="4">
-        <v>146840</v>
-      </c>
-      <c r="I41" s="12">
-        <v>9.3649999999999997E-2</v>
+        <v>152306</v>
+      </c>
+      <c r="I41" s="15">
+        <v>9.7129999999999994E-2</v>
       </c>
       <c r="J41" s="4">
         <v>4</v>
@@ -2851,18 +2843,18 @@
       <c r="K41" s="4">
         <v>2.0969999999999999E-2</v>
       </c>
-      <c r="L41" s="4">
+      <c r="L41" s="14">
+        <f>K41*F41</f>
+        <v>3.7326599999999996</v>
+      </c>
+      <c r="M41" s="5">
         <v>4.8581500000000002</v>
       </c>
-      <c r="M41" s="4">
+      <c r="N41" s="4">
         <v>10</v>
       </c>
-      <c r="N41" s="4" t="s">
+      <c r="O41" s="4" t="s">
         <v>17</v>
-      </c>
-      <c r="O41" s="17">
-        <f t="shared" si="1"/>
-        <v>3.7326599999999996</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- modified the OMPerr function to: 1) take correct error tolerance 2) perform iterations until the min(#dim, dict_size)
- generated results for KSVD with varying dictionary size and varying
epsilon values (#iterations = 50 is fixed)

- included KSVD algorithm in the main function
</commit_message>
<xml_diff>
--- a/output/to_publish/results2.xlsx
+++ b/output/to_publish/results2.xlsx
@@ -991,8 +991,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="H45" sqref="H45"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1096,7 +1096,7 @@
         <v>6.2100000000000002E-3</v>
       </c>
       <c r="L2" s="13">
-        <f>K2*F2</f>
+        <f t="shared" ref="L2:L9" si="0">K2*F2</f>
         <v>0.99981000000000009</v>
       </c>
       <c r="M2" s="7">
@@ -1144,7 +1144,7 @@
         <v>1.3820000000000001E-2</v>
       </c>
       <c r="L3" s="13">
-        <f>K3*F3</f>
+        <f t="shared" si="0"/>
         <v>1.6584000000000001</v>
       </c>
       <c r="M3" s="7">
@@ -1192,7 +1192,7 @@
         <v>0.16406999999999999</v>
       </c>
       <c r="L4" s="13">
-        <f>K4*F4</f>
+        <f t="shared" si="0"/>
         <v>15.586649999999999</v>
       </c>
       <c r="M4" s="7">
@@ -1240,7 +1240,7 @@
         <v>0.12748000000000001</v>
       </c>
       <c r="L5" s="13">
-        <f>K5*F5</f>
+        <f t="shared" si="0"/>
         <v>11.983120000000001</v>
       </c>
       <c r="M5" s="7">
@@ -1288,7 +1288,7 @@
         <v>7.7499999999999999E-3</v>
       </c>
       <c r="L6" s="14">
-        <f>K6*F6</f>
+        <f t="shared" si="0"/>
         <v>0.99975000000000003</v>
       </c>
       <c r="M6" s="5">
@@ -1336,7 +1336,7 @@
         <v>2.4549999999999999E-2</v>
       </c>
       <c r="L7" s="14">
-        <f>K7*F7</f>
+        <f t="shared" si="0"/>
         <v>1.7921499999999999</v>
       </c>
       <c r="M7" s="5">
@@ -1384,7 +1384,7 @@
         <v>0.1091</v>
       </c>
       <c r="L8" s="14">
-        <f>K8*F8</f>
+        <f t="shared" si="0"/>
         <v>3.7094</v>
       </c>
       <c r="M8" s="5">
@@ -1432,7 +1432,7 @@
         <v>0.18879000000000001</v>
       </c>
       <c r="L9" s="14">
-        <f>K9*F9</f>
+        <f t="shared" si="0"/>
         <v>6.4188600000000005</v>
       </c>
       <c r="M9" s="5">
@@ -1497,7 +1497,7 @@
         <v>7.1000000000000002E-4</v>
       </c>
       <c r="L11" s="13">
-        <f>K11*F11</f>
+        <f t="shared" ref="L11:L18" si="1">K11*F11</f>
         <v>1.00607</v>
       </c>
       <c r="M11" s="7">
@@ -1545,7 +1545,7 @@
         <v>2.7100000000000002E-3</v>
       </c>
       <c r="L12" s="13">
-        <f>K12*F12</f>
+        <f t="shared" si="1"/>
         <v>1.7018800000000001</v>
       </c>
       <c r="M12" s="7">
@@ -1593,7 +1593,7 @@
         <v>5.1290000000000002E-2</v>
       </c>
       <c r="L13" s="13">
-        <f>K13*F13</f>
+        <f t="shared" si="1"/>
         <v>17.74634</v>
       </c>
       <c r="M13" s="7">
@@ -1641,7 +1641,7 @@
         <v>5.747E-2</v>
       </c>
       <c r="L14" s="13">
-        <f>K14*F14</f>
+        <f t="shared" si="1"/>
         <v>18.045580000000001</v>
       </c>
       <c r="M14" s="7">
@@ -1689,7 +1689,7 @@
         <v>1.0399999999999999E-3</v>
       </c>
       <c r="L15" s="14">
-        <f>K15*F15</f>
+        <f t="shared" si="1"/>
         <v>1.00464</v>
       </c>
       <c r="M15" s="5">
@@ -1737,7 +1737,7 @@
         <v>6.4700000000000001E-3</v>
       </c>
       <c r="L16" s="14">
-        <f>K16*F16</f>
+        <f t="shared" si="1"/>
         <v>1.8633600000000001</v>
       </c>
       <c r="M16" s="5">
@@ -1785,7 +1785,7 @@
         <v>0.15668000000000001</v>
       </c>
       <c r="L17" s="14">
-        <f>K17*F17</f>
+        <f t="shared" si="1"/>
         <v>13.474480000000002</v>
       </c>
       <c r="M17" s="5">
@@ -1833,7 +1833,7 @@
         <v>0.1757</v>
       </c>
       <c r="L18" s="14">
-        <f>K18*F18</f>
+        <f t="shared" si="1"/>
         <v>13.5289</v>
       </c>
       <c r="M18" s="5">
@@ -1898,7 +1898,7 @@
         <v>3.0400000000000002E-3</v>
       </c>
       <c r="L20" s="13">
-        <f>K20*F20</f>
+        <f t="shared" ref="L20:L27" si="2">K20*F20</f>
         <v>1.0001600000000002</v>
       </c>
       <c r="M20" s="7">
@@ -1946,7 +1946,7 @@
         <v>1.711E-2</v>
       </c>
       <c r="L21" s="13">
-        <f>K21*F21</f>
+        <f t="shared" si="2"/>
         <v>1.81366</v>
       </c>
       <c r="M21" s="7">
@@ -1994,7 +1994,7 @@
         <v>0.39693000000000001</v>
       </c>
       <c r="L22" s="13">
-        <f>K22*F22</f>
+        <f t="shared" si="2"/>
         <v>24.212730000000001</v>
       </c>
       <c r="M22" s="7">
@@ -2042,7 +2042,7 @@
         <v>0.27012000000000003</v>
       </c>
       <c r="L23" s="13">
-        <f>K23*F23</f>
+        <f t="shared" si="2"/>
         <v>16.2072</v>
       </c>
       <c r="M23" s="7">
@@ -2090,7 +2090,7 @@
         <v>4.4999999999999997E-3</v>
       </c>
       <c r="L24" s="14">
-        <f>K24*F24</f>
+        <f t="shared" si="2"/>
         <v>0.99899999999999989</v>
       </c>
       <c r="M24" s="5">
@@ -2138,7 +2138,7 @@
         <v>5.0869999999999999E-2</v>
       </c>
       <c r="L25" s="14">
-        <f>K25*F25</f>
+        <f t="shared" si="2"/>
         <v>1.93306</v>
       </c>
       <c r="M25" s="5">
@@ -2186,7 +2186,7 @@
         <v>0.38769999999999999</v>
       </c>
       <c r="L26" s="14">
-        <f>K26*F26</f>
+        <f t="shared" si="2"/>
         <v>7.7539999999999996</v>
       </c>
       <c r="M26" s="5">
@@ -2234,7 +2234,7 @@
         <v>0.64732999999999996</v>
       </c>
       <c r="L27" s="14">
-        <f>K27*F27</f>
+        <f t="shared" si="2"/>
         <v>11.65194</v>
       </c>
       <c r="M27" s="5">
@@ -2299,7 +2299,7 @@
         <v>1.3799999999999999E-3</v>
       </c>
       <c r="L29" s="13">
-        <f>K29*F29</f>
+        <f t="shared" ref="L29:L34" si="3">K29*F29</f>
         <v>0.99773999999999996</v>
       </c>
       <c r="M29" s="7">
@@ -2347,7 +2347,7 @@
         <v>4.4479999999999999E-2</v>
       </c>
       <c r="L30" s="13">
-        <f>K30*F30</f>
+        <f t="shared" si="3"/>
         <v>8.3177599999999998</v>
       </c>
       <c r="M30" s="7">
@@ -2395,7 +2395,7 @@
         <v>4.3630000000000002E-2</v>
       </c>
       <c r="L31" s="13">
-        <f>K31*F31</f>
+        <f t="shared" si="3"/>
         <v>8.2896999999999998</v>
       </c>
       <c r="M31" s="7">
@@ -2443,7 +2443,7 @@
         <v>2.1099999999999999E-3</v>
       </c>
       <c r="L32" s="14">
-        <f>K32*F32</f>
+        <f t="shared" si="3"/>
         <v>0.99802999999999997</v>
       </c>
       <c r="M32" s="5">
@@ -2491,7 +2491,7 @@
         <v>3.7470000000000003E-2</v>
       </c>
       <c r="L33" s="14">
-        <f>K33*F33</f>
+        <f t="shared" si="3"/>
         <v>2.8477200000000003</v>
       </c>
       <c r="M33" s="5">
@@ -2539,7 +2539,7 @@
         <v>3.5040000000000002E-2</v>
       </c>
       <c r="L34" s="14">
-        <f>K34*F34</f>
+        <f t="shared" si="3"/>
         <v>2.8382400000000003</v>
       </c>
       <c r="M34" s="5">
@@ -2604,7 +2604,7 @@
         <v>6.7000000000000002E-4</v>
       </c>
       <c r="L36" s="13">
-        <f>K36*F36</f>
+        <f t="shared" ref="L36:L41" si="4">K36*F36</f>
         <v>0.99763000000000002</v>
       </c>
       <c r="M36" s="7">
@@ -2652,7 +2652,7 @@
         <v>2.0129999999999999E-2</v>
       </c>
       <c r="L37" s="13">
-        <f>K37*F37</f>
+        <f t="shared" si="4"/>
         <v>8.1727799999999995</v>
       </c>
       <c r="M37" s="7">
@@ -2700,7 +2700,7 @@
         <v>2.095E-2</v>
       </c>
       <c r="L38" s="13">
-        <f>K38*F38</f>
+        <f t="shared" si="4"/>
         <v>8.2333499999999997</v>
       </c>
       <c r="M38" s="7">
@@ -2748,7 +2748,7 @@
         <v>9.3000000000000005E-4</v>
       </c>
       <c r="L39" s="14">
-        <f>K39*F39</f>
+        <f t="shared" si="4"/>
         <v>0.99696000000000007</v>
       </c>
       <c r="M39" s="5">
@@ -2796,7 +2796,7 @@
         <v>1.5570000000000001E-2</v>
       </c>
       <c r="L40" s="14">
-        <f>K40*F40</f>
+        <f t="shared" si="4"/>
         <v>2.8181700000000003</v>
       </c>
       <c r="M40" s="5">
@@ -2844,7 +2844,7 @@
         <v>2.0969999999999999E-2</v>
       </c>
       <c r="L41" s="14">
-        <f>K41*F41</f>
+        <f t="shared" si="4"/>
         <v>3.7326599999999996</v>
       </c>
       <c r="M41" s="5">

</xml_diff>